<commit_message>
finalized the MoM and YoY excel sheets.
</commit_message>
<xml_diff>
--- a/yfinance/output_YOY_total_Value.xlsx
+++ b/yfinance/output_YOY_total_Value.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerpapenfuss/finance_testing/alpaca_api/yfinance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{28CF5DBB-8096-734A-8AC1-75A78B39F007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE7903E-28FF-BA4D-B7F8-E5CB05AD64D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{468CAF37-4B12-1946-9228-EA40FEC6A74A}"/>
+    <workbookView xWindow="5260" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{468CAF37-4B12-1946-9228-EA40FEC6A74A}"/>
   </bookViews>
   <sheets>
     <sheet name="output_YOY" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="1122">
   <si>
     <t>Ticker</t>
   </si>
@@ -3382,13 +3395,10 @@
     <t>Portfolio_Weight_Percent</t>
   </si>
   <si>
-    <t>Total losses 100k</t>
-  </si>
-  <si>
-    <t>Total Losses 1M</t>
-  </si>
-  <si>
-    <t>Total Losses 100K 10% threshold</t>
+    <t>$100k</t>
+  </si>
+  <si>
+    <t>$1M</t>
   </si>
 </sst>
 </file>
@@ -4254,7 +4264,7 @@
   <dimension ref="A1:O251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4326,12 +4336,6 @@
         <f>ROUND(100000*H2*I2*0.01*0.01, 2)</f>
         <v>-109.69</v>
       </c>
-      <c r="N2" t="s">
-        <v>1120</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1121</v>
-      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -4365,14 +4369,6 @@
         <f t="shared" ref="J3:J61" si="0">ROUND(100000*H3*I3*0.01*0.01, 2)</f>
         <v>-69.489999999999995</v>
       </c>
-      <c r="N3">
-        <f>SUM(J2:J61)</f>
-        <v>-853.13999999999976</v>
-      </c>
-      <c r="O3">
-        <f>SUM(J2:J61)*10</f>
-        <v>-8531.3999999999978</v>
-      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -4473,7 +4469,10 @@
         <v>-12.5</v>
       </c>
       <c r="N6" t="s">
-        <v>1122</v>
+        <v>1120</v>
+      </c>
+      <c r="O6" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>